<commit_message>
Split merging into slow and eddy
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Marginal distribution sampling</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>RH</t>
+  </si>
+  <si>
+    <t>Berge</t>
+  </si>
+  <si>
+    <t>delta_T</t>
+  </si>
+  <si>
+    <t>Berge + Thermistor</t>
   </si>
 </sst>
 </file>
@@ -387,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,8 +443,12 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -446,8 +459,23 @@
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Include thermistors in gapfilling
Add random error calculation in EddyPro
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Berge_MDS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Marginal distribution sampling</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>Berge</t>
+  </si>
+  <si>
+    <t>Proxy_vars_range_alternative_station</t>
+  </si>
+  <si>
+    <t>water_temp_0m0_Therm2</t>
+  </si>
+  <si>
+    <t>Alternative_station</t>
+  </si>
+  <si>
+    <t>Proxy_vars_subset</t>
+  </si>
+  <si>
+    <t>water_temp_0m4_Therm1</t>
+  </si>
+  <si>
+    <t>water_temp_0m4_Therm2</t>
   </si>
 </sst>
 </file>
@@ -403,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,12 +432,15 @@
     <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -433,13 +454,22 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -452,14 +482,23 @@
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -468,21 +507,33 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -492,10 +543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,13 +554,16 @@
     <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -523,17 +577,25 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -546,17 +608,26 @@
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -565,21 +636,28 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
         <v>3.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change gapfilling indexing system
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Marginal distribution sampling</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>water_temp_0m4_Therm2</t>
+  </si>
+  <si>
+    <t>delta_Tair_Teau</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,14 +482,14 @@
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
@@ -505,13 +508,11 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -521,11 +522,11 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>11</v>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Fix gap filling indexing bug
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Marginal distribution sampling</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>delta_Tair_Teau</t>
+  </si>
+  <si>
+    <t>CH4_flux</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,6 +525,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Solve merging and index issues
Solve merging issues
Add CO2 to gapfilling config
Remove duplicate naming in gapfiling_configuration
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>Marginal distribution sampling</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>CH4_flux</t>
+  </si>
+  <si>
+    <t>CO2_flux</t>
   </si>
 </sst>
 </file>
@@ -539,6 +542,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
       <c r="H5" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Update gap filling methodology
Allows different proxy variables for each variable that should be gap filled
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Marginal distribution sampling</t>
   </si>
@@ -103,6 +103,51 @@
   </si>
   <si>
     <t>CO2_flux</t>
+  </si>
+  <si>
+    <t>LE_proxy_vars</t>
+  </si>
+  <si>
+    <t>LE_proxy_vars_subset</t>
+  </si>
+  <si>
+    <t>LE_proxy_vars_range</t>
+  </si>
+  <si>
+    <t>H_proxy_vars</t>
+  </si>
+  <si>
+    <t>H_proxy_vars_subset</t>
+  </si>
+  <si>
+    <t>H_proxy_vars_range</t>
+  </si>
+  <si>
+    <t>CO2_flux_proxy_vars</t>
+  </si>
+  <si>
+    <t>CO2_flux_proxy_vars_subset</t>
+  </si>
+  <si>
+    <t>CH4_flux_proxy_vars</t>
+  </si>
+  <si>
+    <t>CH4_flux_proxy_vars_subset</t>
+  </si>
+  <si>
+    <t>CO2_flux_proxy_vars_range</t>
+  </si>
+  <si>
+    <t>CH4_flux_proxy_vars_range</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Name: Marginal distribution sampling</t>
+  </si>
+  <si>
+    <t>Reference: Reichtein et al. 2005</t>
   </si>
 </sst>
 </file>
@@ -126,12 +171,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,10 +209,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,127 +502,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8">
+        <v>1</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+      <c r="F4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>3</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7">
+        <v>3</v>
+      </c>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="O5" s="11"/>
+      <c r="P5" s="11" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Improve missing rain handling
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Berge_MDS" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
-  <si>
-    <t>Marginal distribution sampling</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t>LE</t>
   </si>
@@ -36,33 +33,15 @@
     <t>H</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Reichtein et al. 2005</t>
-  </si>
-  <si>
     <t>Vars_to_fill</t>
   </si>
   <si>
-    <t>Proxy_vars</t>
-  </si>
-  <si>
-    <t>Proxy_vars_range</t>
-  </si>
-  <si>
     <t>wind_speed_05103</t>
   </si>
   <si>
     <t>air_relativeHumidity</t>
   </si>
   <si>
-    <t>air_temp_HMP45C</t>
-  </si>
-  <si>
     <t>water_temp_0m0_Therm1</t>
   </si>
   <si>
@@ -72,24 +51,15 @@
     <t>Proxy_vars_alternative_station</t>
   </si>
   <si>
-    <t>Proxy_precip_station</t>
-  </si>
-  <si>
     <t>Berge</t>
   </si>
   <si>
-    <t>Proxy_vars_range_alternative_station</t>
-  </si>
-  <si>
     <t>water_temp_0m0_Therm2</t>
   </si>
   <si>
     <t>Alternative_station</t>
   </si>
   <si>
-    <t>Proxy_vars_subset</t>
-  </si>
-  <si>
     <t>water_temp_0m4_Therm1</t>
   </si>
   <si>
@@ -148,6 +118,12 @@
   </si>
   <si>
     <t>Reference: Reichtein et al. 2005</t>
+  </si>
+  <si>
+    <t>wind_speed_sonic</t>
+  </si>
+  <si>
+    <t>precip_TB4</t>
   </si>
 </sst>
 </file>
@@ -504,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,188 +506,194 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="L1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="O1" s="9" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5">
         <v>3.5</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H2" s="8">
         <v>3.5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="K2" s="5">
         <v>3.5</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="N2" s="8">
         <v>3.5</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8">
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5">
         <v>1</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8">
         <v>1</v>
       </c>
-      <c r="O3" s="11"/>
+      <c r="O3" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="P3" s="11" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
         <v>3</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7">
         <v>3</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4">
         <v>3</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7">
         <v>3</v>
       </c>
-      <c r="O4" s="11"/>
+      <c r="O4" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="P4" s="11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="P5" s="11" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -739,122 +721,210 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>3</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="M4" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>3.5</v>
-      </c>
+      <c r="M6" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve filtering and gap filling
Update Berge eddyPro metadata / add diagnostic
Update Berge gapfilling configuration based on Reinstein for carbon
Reduce bandpass for LE, H, CO2, and CH4
Remove spikes after other criteria are applied
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Berge_MDS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t>LE</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>precip_TB4</t>
+  </si>
+  <si>
+    <t>rad_shortwave_down_CNR4</t>
+  </si>
+  <si>
+    <t>air_temp</t>
+  </si>
+  <si>
+    <t>air_vpd</t>
+  </si>
+  <si>
+    <t>water_temp_surface</t>
   </si>
 </sst>
 </file>
@@ -480,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,19 +592,19 @@
         <v>3.5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="K2" s="5">
-        <v>3.5</v>
+        <v>50</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="N2" s="8">
         <v>3.5</v>
@@ -626,11 +638,11 @@
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>3</v>
@@ -665,18 +677,11 @@
         <v>3</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4">
-        <v>3</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>6</v>
@@ -723,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Convert the code to a package
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Berge_MDS" sheetId="1" r:id="rId1"/>
     <sheet name="Reservoir_MDS" sheetId="2" r:id="rId2"/>
+    <sheet name="Foret_ouest_MDS" sheetId="3" r:id="rId3"/>
+    <sheet name="Foret_est_MDS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="38">
   <si>
     <t>LE</t>
   </si>
@@ -136,6 +138,9 @@
   </si>
   <si>
     <t>water_temp_surface</t>
+  </si>
+  <si>
+    <t>Foret_ouest</t>
   </si>
 </sst>
 </file>
@@ -492,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,13 +821,13 @@
         <v>3.5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="K2" s="5">
-        <v>3.5</v>
+        <v>50</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>6</v>
@@ -853,11 +858,11 @@
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>6</v>
@@ -885,11 +890,11 @@
         <v>3</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>6</v>
@@ -911,6 +916,378 @@
         <v>8</v>
       </c>
       <c r="M6" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="8">
+        <v>50</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <v>500</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>500</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="8">
+        <v>50</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <v>500</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>500</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>500</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Forest_stations and Water_stations virtual stations
The data from the original stations (Berge, Reservoir, Foret_ouest, Foret_est) remain unchanged. Only the Forest_stations and Water_stations undergo data merging and important corrections.
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Berge_MDS" sheetId="1" r:id="rId1"/>
-    <sheet name="Reservoir_MDS" sheetId="2" r:id="rId2"/>
-    <sheet name="Foret_ouest_MDS" sheetId="3" r:id="rId3"/>
-    <sheet name="Foret_est_MDS" sheetId="4" r:id="rId4"/>
+    <sheet name="Foret_ouest_MDS" sheetId="3" r:id="rId2"/>
+    <sheet name="Foret_est_MDS" sheetId="4" r:id="rId3"/>
+    <sheet name="Forest_stations_MDS" sheetId="5" r:id="rId4"/>
+    <sheet name="Reservoir_MDS" sheetId="2" r:id="rId5"/>
+    <sheet name="Water_stations_MDS" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="38">
   <si>
     <t>LE</t>
   </si>
@@ -497,9 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -731,11 +731,545 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="8">
+        <v>50</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <v>500</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>500</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="8">
+        <v>50</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <v>500</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>500</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>500</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="8">
+        <v>50</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <v>500</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>500</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -941,30 +1475,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -998,8 +1535,23 @@
       <c r="K1" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1007,22 +1559,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5">
-        <v>50</v>
+        <v>3.5</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="H2" s="8">
-        <v>50</v>
+        <v>3.5</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>33</v>
@@ -1033,8 +1585,23 @@
       <c r="K2" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1042,18 +1609,18 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>34</v>
@@ -1062,24 +1629,37 @@
       <c r="K3" s="5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8">
+        <v>1</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
-        <v>500</v>
+        <v>3</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7">
-        <v>500</v>
+        <v>3</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>35</v>
@@ -1088,224 +1668,39 @@
       <c r="K4" s="4">
         <v>500</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E15" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="5">
-        <v>50</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="8">
-        <v>50</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="5">
-        <v>50</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4">
-        <v>500</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7">
-        <v>500</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4">
-        <v>500</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E15" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add gapfilling for energy balance corrected flux
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anthi182\Documents\GitHub\Ro2_data_worflow\Config\GapFillingConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A78169A-FA26-4A6D-866D-75EC1D183C81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B46FAD0-3DDD-42DA-A54B-DB43BB4A6B27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forest_stations_MDS" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="48">
   <si>
     <t>LE</t>
   </si>
@@ -150,6 +150,30 @@
   </si>
   <si>
     <t>water_temp_sfc</t>
+  </si>
+  <si>
+    <t>LE_corr_proxy_vars</t>
+  </si>
+  <si>
+    <t>LE_corr_proxy_vars_subset</t>
+  </si>
+  <si>
+    <t>LE_corr_proxy_vars_range</t>
+  </si>
+  <si>
+    <t>H_corr_proxy_vars</t>
+  </si>
+  <si>
+    <t>H_corr_proxy_vars_subset</t>
+  </si>
+  <si>
+    <t>H_corr_proxy_vars_range</t>
+  </si>
+  <si>
+    <t>LE_corr</t>
+  </si>
+  <si>
+    <t>H_corr</t>
   </si>
 </sst>
 </file>
@@ -504,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,9 +548,13 @@
     <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -569,8 +597,26 @@
       <c r="N1" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -613,8 +659,26 @@
       <c r="N2" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>50</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -649,8 +713,22 @@
       <c r="N3" s="7">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -682,22 +760,46 @@
       <c r="N4" s="7">
         <v>500</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4">
+        <v>500</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E15" s="2"/>
     </row>
   </sheetData>
@@ -707,10 +809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,9 +831,15 @@
     <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -774,8 +882,26 @@
       <c r="N1" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -818,8 +944,26 @@
       <c r="N2" s="8">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="8">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -854,8 +998,22 @@
       <c r="N3" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5">
+        <v>1</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -880,27 +1038,51 @@
       <c r="K4" s="4">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4">
+        <v>3</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E15" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix CH4 gap filling config for forest stations
</commit_message>
<xml_diff>
--- a/Config/GapFillingConfig/gapfilling_configuration.xlsx
+++ b/Config/GapFillingConfig/gapfilling_configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anthi182\Documents\GitHub\Ro2_data_worflow\Config\GapFillingConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/anthi182_ulaval_ca/Documents/Documents/GitHub/Ro2_data_worflow/Config/GapFillingConfig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B46FAD0-3DDD-42DA-A54B-DB43BB4A6B27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9B46FAD0-3DDD-42DA-A54B-DB43BB4A6B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7E7AEED-C72F-4763-9505-1BFB19C1DD60}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forest_stations_MDS" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="48">
   <si>
     <t>LE</t>
   </si>
@@ -531,30 +531,30 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -616,7 +616,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -678,7 +678,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -728,7 +728,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -775,31 +775,36 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E15" s="2"/>
     </row>
   </sheetData>
@@ -815,31 +820,31 @@
       <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -901,7 +906,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -963,7 +968,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1013,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1053,36 +1058,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E15" s="2"/>
     </row>
   </sheetData>
@@ -1098,27 +1103,27 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1168,7 +1173,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1218,7 +1223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1260,7 +1265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1292,7 +1297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -1303,21 +1308,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="E15" s="2"/>
     </row>
   </sheetData>
@@ -1334,23 +1339,23 @@
       <selection activeCell="L1" sqref="L1:N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1394,7 +1399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1438,7 +1443,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1474,7 +1479,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1507,26 +1512,26 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E15" s="2"/>
     </row>
   </sheetData>
@@ -1541,22 +1546,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1597,7 +1602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1638,7 +1643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1673,7 +1678,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1705,7 +1710,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L5" s="10" t="s">
         <v>37</v>
       </c>
@@ -1713,21 +1718,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E15" s="2"/>
     </row>
   </sheetData>
@@ -1741,24 +1746,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1799,7 +1804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1840,7 +1845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1875,7 +1880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1907,7 +1912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L5" s="10" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1920,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L6" s="10" t="s">
         <v>8</v>
       </c>
@@ -1923,21 +1928,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E15" s="2"/>
     </row>
   </sheetData>

</xml_diff>